<commit_message>
added capwap and pda
</commit_message>
<xml_diff>
--- a/Draft Excel Codelists/capwap.xlsx
+++ b/Draft Excel Codelists/capwap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcutts/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7D2DB26-0F63-9A47-89C8-8894231018B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858A7CE7-4B02-D647-B757-4130D25B4671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57020" yWindow="2080" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68900" yWindow="5300" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -810,9 +810,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>pda_properties</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -1006,6 +1003,9 @@
   </si>
   <si>
     <t>DIGGS Measurement Properties for CAPWAP</t>
+  </si>
+  <si>
+    <t>capwap_properties</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1185,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1231,15 +1231,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1843,8 +1834,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1888,10 +1879,10 @@
         <v>233</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>257</v>
+        <v>322</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>234</v>
@@ -1960,16 +1951,16 @@
         <v/>
       </c>
       <c r="B2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C2" t="s">
         <v>227</v>
       </c>
       <c r="D2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F2" t="s">
         <v>251</v>
@@ -1977,371 +1968,356 @@
       <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="str">
+      <c r="A3" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B2830,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C3" t="s">
         <v>269</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>270</v>
       </c>
-      <c r="D3" t="s">
-        <v>271</v>
-      </c>
       <c r="E3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F3" t="s">
-        <v>264</v>
-      </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+        <v>263</v>
+      </c>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="str">
+      <c r="A4" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B4,AssociatedElements!B$2:B2831,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" t="s">
         <v>272</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>273</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" t="s">
         <v>274</v>
       </c>
-      <c r="E4" t="s">
-        <v>261</v>
-      </c>
-      <c r="F4" t="s">
-        <v>275</v>
-      </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="str">
+      <c r="A5" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B2832,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" t="s">
         <v>276</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>277</v>
       </c>
-      <c r="D5" t="s">
-        <v>278</v>
-      </c>
       <c r="E5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F5" t="s">
-        <v>260</v>
-      </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
+        <v>259</v>
+      </c>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="str">
+      <c r="A6" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B2833,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" t="s">
         <v>279</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>280</v>
       </c>
-      <c r="D6" t="s">
-        <v>281</v>
-      </c>
       <c r="E6" t="s">
+        <v>260</v>
+      </c>
+      <c r="F6" t="s">
         <v>261</v>
       </c>
-      <c r="F6" t="s">
-        <v>262</v>
-      </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="str">
+      <c r="A7" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B2834,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7" t="s">
         <v>282</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>283</v>
       </c>
-      <c r="D7" t="s">
-        <v>284</v>
-      </c>
       <c r="E7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F7" t="s">
-        <v>283</v>
-      </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
+        <v>282</v>
+      </c>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="str">
+      <c r="A8" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B2835,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" t="s">
         <v>285</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>286</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>260</v>
+      </c>
+      <c r="F8" t="s">
         <v>287</v>
       </c>
-      <c r="E8" t="s">
-        <v>261</v>
-      </c>
-      <c r="F8" t="s">
-        <v>288</v>
-      </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="str">
+      <c r="A9" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B9,AssociatedElements!B$2:B2836,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" t="s">
         <v>289</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>290</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>291</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>292</v>
       </c>
-      <c r="F9" t="s">
-        <v>293</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="str">
+      <c r="A10" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B2837,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C10" t="s">
         <v>294</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>295</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>296</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>297</v>
       </c>
-      <c r="F10" t="s">
-        <v>298</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="str">
+      <c r="A11" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B2838,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B11" t="s">
+        <v>298</v>
+      </c>
+      <c r="C11" t="s">
         <v>299</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>300</v>
       </c>
-      <c r="D11" t="s">
-        <v>301</v>
-      </c>
       <c r="E11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F11" t="s">
-        <v>265</v>
-      </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="23"/>
+        <v>264</v>
+      </c>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="str">
+      <c r="A12" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B12,AssociatedElements!B$2:B2839,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B12" t="s">
+        <v>301</v>
+      </c>
+      <c r="C12" t="s">
         <v>302</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>303</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>260</v>
+      </c>
+      <c r="F12" t="s">
         <v>304</v>
       </c>
-      <c r="E12" t="s">
-        <v>261</v>
-      </c>
-      <c r="F12" t="s">
-        <v>305</v>
-      </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="23"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="str">
+      <c r="A13" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B2840,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B13" t="s">
+        <v>305</v>
+      </c>
+      <c r="C13" t="s">
         <v>306</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>307</v>
       </c>
-      <c r="D13" t="s">
-        <v>308</v>
-      </c>
       <c r="E13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F13" t="s">
-        <v>263</v>
-      </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
+        <v>262</v>
+      </c>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="str">
+      <c r="A14" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B14,AssociatedElements!B$2:B2841,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C14" t="s">
         <v>309</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>310</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>260</v>
+      </c>
+      <c r="F14" t="s">
         <v>311</v>
       </c>
-      <c r="E14" t="s">
-        <v>261</v>
-      </c>
-      <c r="F14" t="s">
-        <v>312</v>
-      </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="str">
+      <c r="A15" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B2842,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B15" t="s">
+        <v>312</v>
+      </c>
+      <c r="C15" t="s">
         <v>313</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>314</v>
       </c>
-      <c r="D15" t="s">
-        <v>315</v>
-      </c>
       <c r="E15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F15" t="s">
-        <v>264</v>
-      </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23"/>
+        <v>263</v>
+      </c>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="str">
+      <c r="A16" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B16,AssociatedElements!B$2:B2843,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B16" t="s">
+        <v>315</v>
+      </c>
+      <c r="C16" t="s">
         <v>316</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>317</v>
       </c>
-      <c r="D16" t="s">
-        <v>318</v>
-      </c>
       <c r="E16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F16" t="s">
-        <v>266</v>
-      </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="23"/>
-    </row>
-    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="str">
+        <v>265</v>
+      </c>
+      <c r="G16" s="19"/>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="str">
         <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2844,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B17" t="s">
+        <v>318</v>
+      </c>
+      <c r="C17" t="s">
         <v>319</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>320</v>
       </c>
-      <c r="D17" t="s">
-        <v>321</v>
-      </c>
       <c r="E17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F17" t="s">
-        <v>267</v>
-      </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="23"/>
-    </row>
-    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="14" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="16" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B23" s="20" t="s">
         <v>256</v>
       </c>
@@ -2373,7 +2349,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
@@ -2406,7 +2382,7 @@
         <v/>
       </c>
       <c r="B2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>250</v>
@@ -2421,7 +2397,7 @@
         <v/>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>250</v>
@@ -2436,7 +2412,7 @@
         <v/>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>250</v>
@@ -2451,7 +2427,7 @@
         <v/>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>250</v>
@@ -2466,7 +2442,7 @@
         <v/>
       </c>
       <c r="B6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>250</v>
@@ -2481,7 +2457,7 @@
         <v/>
       </c>
       <c r="B7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>250</v>
@@ -2496,7 +2472,7 @@
         <v/>
       </c>
       <c r="B8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>250</v>
@@ -2511,7 +2487,7 @@
         <v/>
       </c>
       <c r="B9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>250</v>
@@ -2526,7 +2502,7 @@
         <v/>
       </c>
       <c r="B10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>250</v>
@@ -2541,7 +2517,7 @@
         <v/>
       </c>
       <c r="B11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>250</v>
@@ -2556,7 +2532,7 @@
         <v/>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>250</v>
@@ -2571,7 +2547,7 @@
         <v/>
       </c>
       <c r="B13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>250</v>
@@ -2586,7 +2562,7 @@
         <v/>
       </c>
       <c r="B14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>250</v>
@@ -2601,7 +2577,7 @@
         <v/>
       </c>
       <c r="B15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>250</v>
@@ -2616,7 +2592,7 @@
         <v/>
       </c>
       <c r="B16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>250</v>
@@ -2631,7 +2607,7 @@
         <v/>
       </c>
       <c r="B17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>250</v>

</xml_diff>